<commit_message>
Massive updates to monsoon variability
</commit_message>
<xml_diff>
--- a/inst/extdata/geo_adjustments.xlsx
+++ b/inst/extdata/geo_adjustments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\Arid-Land-Hydrology\R\WatershedElements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D192BCC-1A55-4495-A47D-547FEA5FCB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281CE90B-7CAA-4AC3-99B5-8C37D2D65229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{526F9EC4-21AA-4855-B4F9-E5AF89EAD13B}"/>
+    <workbookView xWindow="13836" yWindow="0" windowWidth="9300" windowHeight="12336" xr2:uid="{526F9EC4-21AA-4855-B4F9-E5AF89EAD13B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -297,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -449,17 +449,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81002B4A-1A44-4C4D-BCC3-C55F6A374BBA}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -487,7 +489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -501,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -515,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -529,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -543,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -557,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -571,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -585,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -599,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -613,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -627,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -641,60 +643,60 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14">
-        <v>0.85</v>
+        <v>0.1</v>
       </c>
       <c r="C14">
         <v>0.9</v>
       </c>
       <c r="D14">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15">
-        <v>0.85</v>
+        <v>0.1</v>
       </c>
       <c r="C15">
         <v>0.9</v>
       </c>
       <c r="D15">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16">
-        <v>0.85</v>
+        <v>0.1</v>
       </c>
       <c r="C16">
         <v>0.9</v>
       </c>
       <c r="D16">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17">
-        <v>0.85</v>
+        <v>0.1</v>
       </c>
       <c r="C17">
         <v>0.9</v>
       </c>
       <c r="D17">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjustments to infiltration parameters
</commit_message>
<xml_diff>
--- a/inst/extdata/geo_adjustments.xlsx
+++ b/inst/extdata/geo_adjustments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\desertHydro\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PackageDev\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281CE90B-7CAA-4AC3-99B5-8C37D2D65229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A42E5FB-EE10-401C-939A-5E12F5BF1B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13836" yWindow="0" windowWidth="9300" windowHeight="12336" xr2:uid="{526F9EC4-21AA-4855-B4F9-E5AF89EAD13B}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{526F9EC4-21AA-4855-B4F9-E5AF89EAD13B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,18 +450,18 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -503,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -517,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -587,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -629,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -643,60 +643,60 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C14">
         <v>0.9</v>
       </c>
       <c r="D14">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C15">
         <v>0.9</v>
       </c>
       <c r="D15">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C16">
         <v>0.9</v>
       </c>
       <c r="D16">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C17">
         <v>0.9</v>
       </c>
       <c r="D17">
-        <v>0.75</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove garbage calls and replace terra::values with terra::global
</commit_message>
<xml_diff>
--- a/inst/extdata/geo_adjustments.xlsx
+++ b/inst/extdata/geo_adjustments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PackageDev\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A42E5FB-EE10-401C-939A-5E12F5BF1B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70AC139-AF9E-4C02-9AFC-B1FDB0CF43E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{526F9EC4-21AA-4855-B4F9-E5AF89EAD13B}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="D13">
         <v>1.05</v>

</xml_diff>